<commit_message>
Bugfix and small changes in cookies business logic; Docker and Docker Compose configs
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veceloe/GitHub/pizzatime/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veceloe/GitHub/pizzatime-main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F277A066-8B6E-F346-9443-927931BC3325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A278E-4B0F-9647-9974-11019282023F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="27140" windowHeight="13400" xr2:uid="{C96F5903-2B22-694E-A45D-AAF782F1CF75}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C96F5903-2B22-694E-A45D-AAF782F1CF75}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Тип</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>https://www.google.com/url?sa=i&amp;url=https%3A%2F%2Flavka.yandex.ru%2F21621%2Fgood%2Fb26cdd6389d24eb9be0605306a0c7730000200010000&amp;psig=AOvVaw38hGrhUAimeY5BMtzZ_pld&amp;ust=1671932712759000&amp;source=images&amp;cd=vfe&amp;ved=0CA8QjRxqFwoTCPipje2QkfwCFQAAAAAdAAAAABAE</t>
+  </si>
+  <si>
+    <t>Кофе</t>
+  </si>
+  <si>
+    <t>Американо или эспрессо на выбор, 0.2л</t>
+  </si>
+  <si>
+    <t>https://www.pngmart.com/files/21/Coffee-Cup-PNG-Isolated-Pic.png</t>
+  </si>
+  <si>
+    <t>Зеленый или черный на выбор</t>
+  </si>
+  <si>
+    <t>Чай Lipton</t>
+  </si>
+  <si>
+    <t>https://nnjfood.ru/upload/iblock/9dc/ce0wwpjev5mcg1qzbst7v562jrbs6cs3.jpg</t>
   </si>
 </sst>
 </file>
@@ -453,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F9EF54-1C3A-2C4A-8114-AB195C1C6718}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,6 +570,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>